<commit_message>
Add the option to include a storm water effieciency parameter
</commit_message>
<xml_diff>
--- a/ProjectArea_ModelName_Pluvial_Parameters.xlsx
+++ b/ProjectArea_ModelName_Pluvial_Parameters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sputnam\Desktop\PFRA_Production\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sputnam\Documents\GitHub\pfra-hydromet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22968" windowHeight="9120" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22968" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Pluvial_Domain" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Shapefile</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>P01_2D_Domain.shp</t>
+  </si>
+  <si>
+    <t>SW Efficiency</t>
   </si>
 </sst>
 </file>
@@ -880,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B2:B4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -894,10 +897,11 @@
     <col min="4" max="4" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -917,10 +921,13 @@
         <v>16</v>
       </c>
       <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -939,8 +946,11 @@
       <c r="F2">
         <v>2.2031999999999998</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -954,7 +964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -972,6 +982,9 @@
       </c>
       <c r="F4">
         <v>1.5</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -983,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18:D19"/>
     </sheetView>
   </sheetViews>

</xml_diff>